<commit_message>
[Add] new exccel outputs
</commit_message>
<xml_diff>
--- a/docs/_static/INSaFLU_current_outputs_15_01_2018.xlsx
+++ b/docs/_static/INSaFLU_current_outputs_15_01_2018.xlsx
@@ -1149,7 +1149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1261,6 +1261,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1276,11 +1277,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1305,7 +1301,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1677,7 +1678,7 @@
       <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:5" s="41" customFormat="1" ht="26.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="43" t="s">
         <v>82</v>
       </c>
       <c r="B2" s="17"/>
@@ -1707,7 +1708,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="45" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -1724,7 +1725,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A6" s="45"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="20" t="s">
         <v>9</v>
       </c>
@@ -1739,7 +1740,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" customHeight="1">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="20" t="s">
         <v>6</v>
       </c>
@@ -1771,7 +1772,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -1788,7 +1789,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="64.5" customHeight="1">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="20" t="s">
         <v>16</v>
       </c>
@@ -1803,7 +1804,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="34.5">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="22" t="s">
         <v>52</v>
       </c>
@@ -1818,7 +1819,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="34.5">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="22" t="s">
         <v>53</v>
       </c>
@@ -1833,7 +1834,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="50.25" customHeight="1">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="23" t="s">
         <v>73</v>
       </c>
@@ -1866,36 +1867,36 @@
     </row>
     <row r="15" spans="1:5" ht="31.5">
       <c r="A15" s="14"/>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="49" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31.5">
       <c r="A16" s="14"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="52"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="49"/>
+      <c r="E16" s="57"/>
     </row>
     <row r="17" spans="1:5" ht="33" customHeight="1">
       <c r="A17" s="14"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="53"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="50"/>
+      <c r="E17" s="58"/>
     </row>
     <row r="18" spans="1:5" ht="35.25" customHeight="1">
       <c r="A18" s="14"/>
@@ -1988,7 +1989,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="42" t="s">
@@ -2000,12 +2001,12 @@
       <c r="D24" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="55" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="193.5" customHeight="1" thickBot="1">
-      <c r="A25" s="47"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="26" t="s">
         <v>78</v>
       </c>
@@ -2015,7 +2016,7 @@
       <c r="D25" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="58"/>
+      <c r="E25" s="56"/>
     </row>
     <row r="26" spans="1:5" ht="66.75" customHeight="1" thickBot="1">
       <c r="A26" s="16" t="s">
@@ -2035,12 +2036,12 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="50.25" customHeight="1">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="8"/>
     </row>
   </sheetData>

</xml_diff>